<commit_message>
creating a new branch
</commit_message>
<xml_diff>
--- a/TestData/Calendar.xlsx
+++ b/TestData/Calendar.xlsx
@@ -388,7 +388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -403,6 +403,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -713,8 +714,8 @@
   </sheetPr>
   <dimension ref="A1:AZ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,10 +1505,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="12" t="s">
         <v>95</v>
       </c>
       <c r="E9" s="4"/>

</xml_diff>

<commit_message>
UserAdministration class with create user
</commit_message>
<xml_diff>
--- a/TestData/Calendar.xlsx
+++ b/TestData/Calendar.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AB588B-3B47-4B5D-BFE8-566E33E179CA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927B4C78-6D16-4ED1-A611-1B0C9437121E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24890" windowHeight="10670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,14 +12,14 @@
     <sheet name="KEEP_REFER" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MAIN!$A$1:$AP$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MAIN!$A$1:$AP$11</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="112">
   <si>
     <t>ID</t>
   </si>
@@ -310,6 +310,51 @@
   </si>
   <si>
     <t>ICCID</t>
+  </si>
+  <si>
+    <t>USERGROUP</t>
+  </si>
+  <si>
+    <t>FIRSTNAME</t>
+  </si>
+  <si>
+    <t>MIDDLENAME</t>
+  </si>
+  <si>
+    <t>LASTNAME</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>PHONE</t>
+  </si>
+  <si>
+    <t>99999999</t>
+  </si>
+  <si>
+    <t>test@amdocs.com</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Carrier User</t>
+  </si>
+  <si>
+    <t>TR0001</t>
+  </si>
+  <si>
+    <t>COMPANY</t>
+  </si>
+  <si>
+    <t>AT &amp; T Mobility, USA (10007)</t>
+  </si>
+  <si>
+    <t>UserAdministrationRoc</t>
+  </si>
+  <si>
+    <t>UserAdministrationCarrier</t>
   </si>
 </sst>
 </file>
@@ -746,10 +791,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:AZ10"/>
+  <dimension ref="A1:AZ14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView tabSelected="1" topLeftCell="K3" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1264,7 +1309,7 @@
     </row>
     <row r="6" spans="1:52" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
@@ -1286,38 +1331,30 @@
         <v>60</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>87</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
@@ -1355,57 +1392,49 @@
       <c r="AZ6" s="3"/>
     </row>
     <row r="7" spans="1:52" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
-        <v>6</v>
+      <c r="A7" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="7" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>69</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="P7" s="11">
-        <v>999999999999999</v>
-      </c>
-      <c r="Q7" s="11">
-        <v>999999999999999</v>
-      </c>
-      <c r="R7" s="11">
-        <v>999999999999999</v>
-      </c>
-      <c r="S7" s="11" t="s">
-        <v>88</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
@@ -1443,8 +1472,8 @@
       <c r="AZ7" s="4"/>
     </row>
     <row r="8" spans="1:52" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
-        <v>7</v>
+      <c r="A8" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
@@ -1466,38 +1495,28 @@
         <v>60</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="S8" s="3" t="s">
-        <v>87</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
@@ -1535,15 +1554,15 @@
       <c r="AZ8" s="3"/>
     </row>
     <row r="9" spans="1:52" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
-        <v>8</v>
+      <c r="A9" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -1554,38 +1573,28 @@
         <v>69</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="P9" s="11">
-        <v>999999999999999</v>
-      </c>
-      <c r="Q9" s="11">
-        <v>999999999999999</v>
-      </c>
-      <c r="R9" s="11">
-        <v>999999999999999</v>
-      </c>
-      <c r="S9" s="11" t="s">
-        <v>88</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="O9" s="4"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
@@ -1622,9 +1631,369 @@
       <c r="AY9" s="4"/>
       <c r="AZ9" s="4"/>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.35">
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+    <row r="10" spans="1:52" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="3"/>
+      <c r="AF10" s="3"/>
+      <c r="AG10" s="3"/>
+      <c r="AH10" s="3"/>
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="3"/>
+      <c r="AK10" s="3"/>
+      <c r="AL10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM10" s="3"/>
+      <c r="AN10" s="3"/>
+      <c r="AO10" s="3"/>
+      <c r="AP10" s="3"/>
+      <c r="AQ10" s="3"/>
+      <c r="AR10" s="3"/>
+      <c r="AS10" s="3"/>
+      <c r="AT10" s="3"/>
+      <c r="AU10" s="3"/>
+      <c r="AV10" s="3"/>
+      <c r="AW10" s="3"/>
+      <c r="AX10" s="3"/>
+      <c r="AY10" s="3"/>
+      <c r="AZ10" s="3"/>
+    </row>
+    <row r="11" spans="1:52" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="P11" s="11">
+        <v>999999999999999</v>
+      </c>
+      <c r="Q11" s="11">
+        <v>999999999999999</v>
+      </c>
+      <c r="R11" s="11">
+        <v>999999999999999</v>
+      </c>
+      <c r="S11" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="4"/>
+      <c r="AB11" s="4"/>
+      <c r="AC11" s="4"/>
+      <c r="AD11" s="4"/>
+      <c r="AE11" s="4"/>
+      <c r="AF11" s="4"/>
+      <c r="AG11" s="4"/>
+      <c r="AH11" s="4"/>
+      <c r="AI11" s="4"/>
+      <c r="AJ11" s="4"/>
+      <c r="AK11" s="4"/>
+      <c r="AL11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM11" s="4"/>
+      <c r="AN11" s="4"/>
+      <c r="AO11" s="4"/>
+      <c r="AP11" s="4"/>
+      <c r="AQ11" s="4"/>
+      <c r="AR11" s="4"/>
+      <c r="AS11" s="4"/>
+      <c r="AT11" s="4"/>
+      <c r="AU11" s="4"/>
+      <c r="AV11" s="4"/>
+      <c r="AW11" s="4"/>
+      <c r="AX11" s="4"/>
+      <c r="AY11" s="4"/>
+      <c r="AZ11" s="4"/>
+    </row>
+    <row r="12" spans="1:52" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="3">
+        <v>7</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
+      <c r="AG12" s="3"/>
+      <c r="AH12" s="3"/>
+      <c r="AI12" s="3"/>
+      <c r="AJ12" s="3"/>
+      <c r="AK12" s="3"/>
+      <c r="AL12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM12" s="3"/>
+      <c r="AN12" s="3"/>
+      <c r="AO12" s="3"/>
+      <c r="AP12" s="3"/>
+      <c r="AQ12" s="3"/>
+      <c r="AR12" s="3"/>
+      <c r="AS12" s="3"/>
+      <c r="AT12" s="3"/>
+      <c r="AU12" s="3"/>
+      <c r="AV12" s="3"/>
+      <c r="AW12" s="3"/>
+      <c r="AX12" s="3"/>
+      <c r="AY12" s="3"/>
+      <c r="AZ12" s="3"/>
+    </row>
+    <row r="13" spans="1:52" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
+        <v>8</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="P13" s="11">
+        <v>999999999999999</v>
+      </c>
+      <c r="Q13" s="11">
+        <v>999999999999999</v>
+      </c>
+      <c r="R13" s="11">
+        <v>999999999999999</v>
+      </c>
+      <c r="S13" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
+      <c r="AA13" s="4"/>
+      <c r="AB13" s="4"/>
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="4"/>
+      <c r="AE13" s="4"/>
+      <c r="AF13" s="4"/>
+      <c r="AG13" s="4"/>
+      <c r="AH13" s="4"/>
+      <c r="AI13" s="4"/>
+      <c r="AJ13" s="4"/>
+      <c r="AK13" s="4"/>
+      <c r="AL13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM13" s="4"/>
+      <c r="AN13" s="4"/>
+      <c r="AO13" s="4"/>
+      <c r="AP13" s="4"/>
+      <c r="AQ13" s="4"/>
+      <c r="AR13" s="4"/>
+      <c r="AS13" s="4"/>
+      <c r="AT13" s="4"/>
+      <c r="AU13" s="4"/>
+      <c r="AV13" s="4"/>
+      <c r="AW13" s="4"/>
+      <c r="AX13" s="4"/>
+      <c r="AY13" s="4"/>
+      <c r="AZ13" s="4"/>
+    </row>
+    <row r="14" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Commit for User Admin
</commit_message>
<xml_diff>
--- a/TestData/Calendar.xlsx
+++ b/TestData/Calendar.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927B4C78-6D16-4ED1-A611-1B0C9437121E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95AC68D0-5FF0-4D28-87F6-F4F24CC6ED15}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24890" windowHeight="10670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -793,8 +793,8 @@
   </sheetPr>
   <dimension ref="A1:AZ14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K3" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="E3" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>